<commit_message>
fix: Convert microampere (uA) to milliampere (mA) for HA compatibility
Home Assistant only accepts 'A' or 'mA' as valid units for current device
class, not 'uA'. This caused warnings for leakage current sensors.

Changes:
- Updated generate_mapping_excel.py to convert uA → mA in mapping (2 locations)
- Added UA_TO_MA_POINTS conversion registry in normalizer.py
- Added value conversion logic (divide by 1000) for affected points
- Regenerated mapping files (xlsx, json)

Affected sensors (2):
- ILeakDcAc (Leakage current DC/AC)
- ILeakDcDc (Leakage current DC/DC)

Values now display in mA (e.g., 6.64 mA instead of 6639.57 uA)

Fixes: #[issue-number]

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/vsn-sunspec-point-mapping.xlsx
+++ b/docs/vsn-sunspec-point-mapping.xlsx
@@ -23629,12 +23629,12 @@
       </c>
       <c r="L252" s="3" t="inlineStr">
         <is>
-          <t>uA</t>
+          <t>mA</t>
         </is>
       </c>
       <c r="M252" s="3" t="inlineStr">
         <is>
-          <t>uA</t>
+          <t>mA</t>
         </is>
       </c>
       <c r="N252" s="3" t="inlineStr">
@@ -23727,12 +23727,12 @@
       </c>
       <c r="L253" s="3" t="inlineStr">
         <is>
-          <t>uA</t>
+          <t>mA</t>
         </is>
       </c>
       <c r="M253" s="3" t="inlineStr">
         <is>
-          <t>uA</t>
+          <t>mA</t>
         </is>
       </c>
       <c r="N253" s="3" t="inlineStr">

</xml_diff>

<commit_message>
feat(mapping): update HA display names and fix data issues
- Updated 20 HA display names for better clarity
  - Datalogger entities: simplified names (WiFi SSID, IP address, etc.)
  - Inverter entities: cleaner names (DC current #1, Alarm status, etc.)
  - Device info: shorter names (Model, Serial Number, Firmware Version)
- Fixed device_class and unit errors:
  - Modbus address: removed incorrect current/A classification
  - Firmware Version: removed incorrect voltage/V classification
  - System timestamp: set as timestamp device_class with diagnostic category
- Fixed generate_mapping_excel.py index errors (column references were off)
- Added update_ha_display_names.py script for bulk display name updates
- Regenerated mapping files with all corrections applied
- Total: 210 mapping entries with proper model assignments

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/vsn-sunspec-point-mapping.xlsx
+++ b/docs/vsn-sunspec-point-mapping.xlsx
@@ -1265,7 +1265,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Current alarm status of the inverter</t>
+          <t>Alarm status</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Booster stage temperature</t>
+          <t>Booster temperature</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -3291,7 +3291,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>Device Modbus address</t>
+          <t>Modbus address</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -3299,19 +3299,9 @@
           <t>Device Info</t>
         </is>
       </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
       <c r="U25" t="inlineStr">
         <is>
           <t>measurement</t>
-        </is>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>current</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -3627,7 +3617,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>DC current measurement for string 1</t>
+          <t>DC current #1</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3744,7 +3734,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>DC current measurement for string 2</t>
+          <t>DC current #2</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -3861,7 +3851,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>DC voltage measurement for string 1</t>
+          <t>DC voltage #1</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3978,7 +3968,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>DC voltage measurement for string 2</t>
+          <t>DC voltage #2</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
@@ -16114,7 +16104,7 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>Device model identifier from common model</t>
+          <t>Model</t>
         </is>
       </c>
       <c r="S134" t="inlineStr">
@@ -16343,7 +16333,7 @@
       </c>
       <c r="R136" t="inlineStr">
         <is>
-          <t>Manufacturer name from device common model</t>
+          <t>Manufacturer</t>
         </is>
       </c>
       <c r="S136" t="inlineStr">
@@ -16791,7 +16781,7 @@
       </c>
       <c r="R140" t="inlineStr">
         <is>
-          <t>Device options and features from common model</t>
+          <t>Options</t>
         </is>
       </c>
       <c r="S140" t="inlineStr">
@@ -17600,7 +17590,7 @@
       </c>
       <c r="R147" t="inlineStr">
         <is>
-          <t>Phase A to neutral voltage measurement</t>
+          <t>Phase Voltage AN</t>
         </is>
       </c>
       <c r="S147" t="inlineStr">
@@ -19467,7 +19457,7 @@
       </c>
       <c r="R163" t="inlineStr">
         <is>
-          <t>Device serial number from common model</t>
+          <t>Serial Number</t>
         </is>
       </c>
       <c r="S163" t="inlineStr">
@@ -20030,6 +20020,16 @@
           <t>measurement</t>
         </is>
       </c>
+      <c r="V168" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="W168" t="inlineStr">
+        <is>
+          <t>diagnostic</t>
+        </is>
+      </c>
       <c r="X168" t="inlineStr">
         <is>
           <t>MAYBE</t>
@@ -21548,7 +21548,7 @@
       </c>
       <c r="R181" t="inlineStr">
         <is>
-          <t>DC bulk capacitor voltage</t>
+          <t>DC capacitor voltage</t>
         </is>
       </c>
       <c r="S181" t="inlineStr">
@@ -21665,7 +21665,7 @@
       </c>
       <c r="R182" t="inlineStr">
         <is>
-          <t>DC bulk mid-point voltage</t>
+          <t>DC mid-point voltage</t>
         </is>
       </c>
       <c r="S182" t="inlineStr">
@@ -21899,7 +21899,7 @@
       </c>
       <c r="R184" t="inlineStr">
         <is>
-          <t>Firmware version from device common model</t>
+          <t>Firmware Version</t>
         </is>
       </c>
       <c r="S184" t="inlineStr">
@@ -21907,19 +21907,9 @@
           <t>Device Info</t>
         </is>
       </c>
-      <c r="T184" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
       <c r="U184" t="inlineStr">
         <is>
           <t>measurement</t>
-        </is>
-      </c>
-      <c r="V184" t="inlineStr">
-        <is>
-          <t>voltage</t>
         </is>
       </c>
       <c r="W184" t="inlineStr">
@@ -24082,7 +24072,7 @@
       </c>
       <c r="R203" t="inlineStr">
         <is>
-          <t>Serial number (datalogger)</t>
+          <t>Serial Number</t>
         </is>
       </c>
       <c r="S203" t="inlineStr">
@@ -24662,7 +24652,7 @@
       </c>
       <c r="R208" t="inlineStr">
         <is>
-          <t>WiFi network name (SSID)</t>
+          <t>WiFi SSID</t>
         </is>
       </c>
       <c r="S208" t="inlineStr">
@@ -24769,7 +24759,7 @@
       </c>
       <c r="R209" t="inlineStr">
         <is>
-          <t>WiFi local IP address</t>
+          <t>IP address</t>
         </is>
       </c>
       <c r="S209" t="inlineStr">
@@ -24983,7 +24973,7 @@
       </c>
       <c r="R211" t="inlineStr">
         <is>
-          <t>Wlan 0 Mode operating mode</t>
+          <t>Wlan 0 mode</t>
         </is>
       </c>
       <c r="S211" t="inlineStr">

</xml_diff>